<commit_message>
Mediciones realizadas... varias... agregando cosas al informe.
</commit_message>
<xml_diff>
--- a/EJ1/Mediciones/Mediciones.xlsx
+++ b/EJ1/Mediciones/Mediciones.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Circuito</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Entrada triangular de 70Hz de 0 a 5V.</t>
   </si>
   <si>
-    <t>Analizar de los .csv</t>
-  </si>
-  <si>
     <t>Sin capacitor de salida</t>
   </si>
   <si>
@@ -96,6 +93,33 @@
   </si>
   <si>
     <t>IOL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notas: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Mediciones realizadas con puntas en x10 para no aumentar la capacidad de los transistores. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Se observa que sería mejor agregar un pull-down para no dejar indefinido el estado de la entrada. </t>
+  </si>
+  <si>
+    <t>* En el primer intento se fallo porque no se estaba haciendo la triangular de 50% y estaba usando mal el Probe</t>
+  </si>
+  <si>
+    <t>* Las corrientes se midieron usando un preset de 2MOhm y se fue variando hasta el punto donde cambia… y se calculó con eso la corriente que sacaba.</t>
+  </si>
+  <si>
+    <t>* Para CMOS IOL lo mejor que pude medir es con una alta impedancia que me sacaba hasta 378mV, no pude bajar mas.</t>
+  </si>
+  <si>
+    <t>* En la medición con una cuadrada para la compuerta MOS, parte de la anormalidad en la entrada es producida por no tener capacitor de desacople.</t>
+  </si>
+  <si>
+    <t>* Suposición: Tener las 4 compuertas NOT, produce un consumo de corriente en la transición de forma conjunta que produce las irregularidades.</t>
+  </si>
+  <si>
+    <t>* Nota las mediciones para ver la corriente fue mejor medirlas con un preset y usando el multimetro de torre para mayor precisión luego medir impedancia de carga con el analizador de impedancias.</t>
   </si>
 </sst>
 </file>
@@ -160,7 +184,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -346,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -363,6 +387,42 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -377,6 +437,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -384,61 +447,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -721,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L2:L3"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,18 +780,18 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="3"/>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="10"/>
-      <c r="J1" s="9" t="s">
+      <c r="I1" s="22"/>
+      <c r="J1" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="10"/>
-      <c r="L1" s="9" t="s">
+      <c r="K1" s="22"/>
+      <c r="L1" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="10"/>
+      <c r="M1" s="22"/>
     </row>
     <row r="2" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -791,243 +827,523 @@
       <c r="K2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="27" t="s">
+      <c r="L2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="M2" s="27" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="6">
+        <v>1.337</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="D3" s="7">
+        <v>4.8940000000000001</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="F3" s="7">
+        <f>D3-B3</f>
+        <v>3.5570000000000004</v>
+      </c>
+      <c r="G3" s="8">
+        <f>C3-E3</f>
+        <v>0.16200000000000003</v>
+      </c>
+      <c r="H3" s="33">
+        <v>5.49E-6</v>
+      </c>
+      <c r="I3" s="32">
+        <v>1.88E-6</v>
+      </c>
+      <c r="J3" s="32">
+        <v>1.37E-6</v>
+      </c>
+      <c r="K3" s="31">
+        <v>6.1199999999999999E-6</v>
+      </c>
+      <c r="L3" s="11">
+        <v>1.438E-5</v>
+      </c>
+      <c r="M3" s="13">
+        <v>4.8809999999999999E-4</v>
+      </c>
+      <c r="N3" s="18" t="s">
         <v>19</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="7"/>
+      <c r="B4" s="6">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0.3085</v>
+      </c>
+      <c r="D4" s="7">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="F4" s="7">
+        <f>D4-B4</f>
+        <v>4.3220000000000001</v>
+      </c>
+      <c r="G4" s="8">
+        <f t="shared" ref="G4:G10" si="0">C4-E4</f>
+        <v>0.29259999999999997</v>
+      </c>
+      <c r="H4" s="33">
+        <v>2.8100000000000002E-6</v>
+      </c>
+      <c r="I4" s="32">
+        <v>5.5000000000000003E-8</v>
+      </c>
+      <c r="J4" s="32">
+        <v>5.7200000000000003E-8</v>
+      </c>
+      <c r="K4" s="31">
+        <v>5.7000000000000005E-7</v>
+      </c>
+      <c r="L4" s="12">
+        <v>1.4569999999999999E-5</v>
+      </c>
+      <c r="M4" s="14">
+        <v>1.312E-5</v>
+      </c>
+      <c r="N4" s="19"/>
     </row>
     <row r="5" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="7"/>
+      <c r="B5" s="6">
+        <v>2.6989999999999998</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1.9394</v>
+      </c>
+      <c r="D5" s="7">
+        <v>4.8928000000000003</v>
+      </c>
+      <c r="E5" s="7">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="F5" s="7">
+        <f t="shared" ref="F5:F10" si="1">D5-B5</f>
+        <v>2.1938000000000004</v>
+      </c>
+      <c r="G5" s="8">
+        <f t="shared" si="0"/>
+        <v>1.8974</v>
+      </c>
+      <c r="H5" s="33">
+        <v>1.5299999999999999E-5</v>
+      </c>
+      <c r="I5" s="32">
+        <v>1.85E-7</v>
+      </c>
+      <c r="J5" s="32">
+        <v>1.7700000000000001E-7</v>
+      </c>
+      <c r="K5" s="31">
+        <v>2.7399999999999999E-5</v>
+      </c>
+      <c r="L5" s="12">
+        <v>1.145E-5</v>
+      </c>
+      <c r="M5" s="14">
+        <v>2.4852000000000001E-4</v>
+      </c>
+      <c r="N5" s="19"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="8"/>
-    </row>
-    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="6">
+        <v>1.7030000000000001</v>
+      </c>
+      <c r="C6" s="7">
+        <v>2.8919999999999999</v>
+      </c>
+      <c r="D6" s="7">
+        <v>4.9377000000000004</v>
+      </c>
+      <c r="E6" s="7">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="F6" s="7">
+        <f t="shared" si="1"/>
+        <v>3.2347000000000001</v>
+      </c>
+      <c r="G6" s="8">
+        <f t="shared" si="0"/>
+        <v>2.8559999999999999</v>
+      </c>
+      <c r="H6" s="33">
+        <v>7.0999999999999998E-7</v>
+      </c>
+      <c r="I6" s="32">
+        <v>7.1999999999999999E-7</v>
+      </c>
+      <c r="J6" s="32">
+        <v>4.1199999999999998E-7</v>
+      </c>
+      <c r="K6" s="31">
+        <v>5.0399999999999996E-7</v>
+      </c>
+      <c r="L6" s="12">
+        <v>1.523E-2</v>
+      </c>
+      <c r="M6" s="14">
+        <v>1.3522999999999999E-4</v>
+      </c>
+      <c r="N6" s="20"/>
+    </row>
+    <row r="7" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="6">
+        <v>1.3180000000000001</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0.25390000000000001</v>
+      </c>
+      <c r="D7" s="7">
+        <v>4.8959999999999999</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0.129</v>
+      </c>
+      <c r="F7" s="7">
+        <f>D7-B7</f>
+        <v>3.5779999999999998</v>
+      </c>
+      <c r="G7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.12490000000000001</v>
+      </c>
+      <c r="H7" s="33">
+        <v>1.1240000000000001E-5</v>
+      </c>
+      <c r="I7" s="32">
+        <v>2.7499999999999999E-6</v>
+      </c>
+      <c r="J7" s="32">
+        <v>2.7999999999999999E-6</v>
+      </c>
+      <c r="K7" s="31">
+        <v>2.9200000000000002E-5</v>
+      </c>
+      <c r="L7" s="12">
+        <v>1.113E-5</v>
+      </c>
+      <c r="M7" s="14">
+        <v>1.1299999999999999E-3</v>
+      </c>
+      <c r="N7" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="7"/>
-    </row>
-    <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="6">
+        <v>0.5585</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.3105</v>
+      </c>
+      <c r="D8" s="7">
+        <v>4.8920000000000003</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1.3899999999999999E-2</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="shared" si="1"/>
+        <v>4.3335000000000008</v>
+      </c>
+      <c r="G8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.29659999999999997</v>
+      </c>
+      <c r="H8" s="33">
+        <v>9.6800000000000005E-6</v>
+      </c>
+      <c r="I8" s="32">
+        <v>7.1999999999999996E-8</v>
+      </c>
+      <c r="J8" s="32">
+        <v>2.0599999999999999E-7</v>
+      </c>
+      <c r="K8" s="31">
+        <v>2.7800000000000001E-5</v>
+      </c>
+      <c r="L8" s="12">
+        <v>1.0180000000000001E-5</v>
+      </c>
+      <c r="M8" s="14">
+        <v>4.9499999999999997E-5</v>
+      </c>
+      <c r="N8" s="19"/>
+    </row>
+    <row r="9" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="7"/>
+      <c r="B9" s="6">
+        <v>2.5289999999999999</v>
+      </c>
+      <c r="C9" s="7">
+        <v>2.1070000000000002</v>
+      </c>
+      <c r="D9" s="7">
+        <v>4.8769999999999998</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1.14E-2</v>
+      </c>
+      <c r="F9" s="7">
+        <f t="shared" si="1"/>
+        <v>2.3479999999999999</v>
+      </c>
+      <c r="G9" s="8">
+        <f t="shared" si="0"/>
+        <v>2.0956000000000001</v>
+      </c>
+      <c r="H9" s="33">
+        <v>2.34E-5</v>
+      </c>
+      <c r="I9" s="32">
+        <v>2.1E-7</v>
+      </c>
+      <c r="J9" s="32">
+        <v>1.8199999999999999E-7</v>
+      </c>
+      <c r="K9" s="31">
+        <v>5.1199999999999998E-5</v>
+      </c>
+      <c r="L9" s="12">
+        <v>1.242E-5</v>
+      </c>
+      <c r="M9" s="14">
+        <v>3.7669999999999997E-5</v>
+      </c>
+      <c r="N9" s="19"/>
     </row>
     <row r="10" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="8"/>
+      <c r="B10" s="6">
+        <v>1.4490000000000001</v>
+      </c>
+      <c r="C10" s="7">
+        <v>2.8260000000000001</v>
+      </c>
+      <c r="D10" s="7">
+        <v>4.9409999999999998</v>
+      </c>
+      <c r="E10" s="7">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="F10" s="7">
+        <f t="shared" si="1"/>
+        <v>3.492</v>
+      </c>
+      <c r="G10" s="8">
+        <f t="shared" si="0"/>
+        <v>2.79</v>
+      </c>
+      <c r="H10" s="33">
+        <v>7.5000000000000002E-7</v>
+      </c>
+      <c r="I10" s="32">
+        <v>7.4499999999999996E-7</v>
+      </c>
+      <c r="J10" s="32">
+        <v>4.34E-7</v>
+      </c>
+      <c r="K10" s="31">
+        <v>5.3200000000000005E-7</v>
+      </c>
+      <c r="L10" s="34">
+        <v>2.129E-2</v>
+      </c>
+      <c r="M10" s="35">
+        <v>1.0169E-4</v>
+      </c>
+      <c r="N10" s="20"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M12" s="17" t="s">
+      <c r="B12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="M12" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="12"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="25"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M13" s="18" t="s">
+      <c r="B13" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="M13" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="14"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="28"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M14" s="19" t="s">
+      <c r="B14" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="M14" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="17"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="8">
+    <mergeCell ref="H1:I1"/>
     <mergeCell ref="M12:P12"/>
     <mergeCell ref="M13:P13"/>
     <mergeCell ref="M14:P14"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="B9:G9"/>
     <mergeCell ref="N3:N6"/>
     <mergeCell ref="N7:N10"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
     <mergeCell ref="J1:K1"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="H5:K5"/>
     <mergeCell ref="L1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ejercicio 1 informe terminado, claramente lo del limite de paginas no me funciona...
</commit_message>
<xml_diff>
--- a/EJ1/Mediciones/Mediciones.xlsx
+++ b/EJ1/Mediciones/Mediciones.xlsx
@@ -370,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -414,6 +414,48 @@
     <xf numFmtId="11" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -431,51 +473,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -759,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B20" sqref="B13:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,16 +855,16 @@
         <f>C3-E3</f>
         <v>0.16200000000000003</v>
       </c>
-      <c r="H3" s="33">
+      <c r="H3" s="18">
         <v>5.49E-6</v>
       </c>
-      <c r="I3" s="32">
+      <c r="I3" s="17">
         <v>1.88E-6</v>
       </c>
-      <c r="J3" s="32">
+      <c r="J3" s="17">
         <v>1.37E-6</v>
       </c>
-      <c r="K3" s="31">
+      <c r="K3" s="16">
         <v>6.1199999999999999E-6</v>
       </c>
       <c r="L3" s="11">
@@ -876,7 +873,7 @@
       <c r="M3" s="13">
         <v>4.8809999999999999E-4</v>
       </c>
-      <c r="N3" s="18" t="s">
+      <c r="N3" s="32" t="s">
         <v>19</v>
       </c>
     </row>
@@ -904,16 +901,16 @@
         <f t="shared" ref="G4:G10" si="0">C4-E4</f>
         <v>0.29259999999999997</v>
       </c>
-      <c r="H4" s="33">
+      <c r="H4" s="18">
         <v>2.8100000000000002E-6</v>
       </c>
-      <c r="I4" s="32">
+      <c r="I4" s="17">
         <v>5.5000000000000003E-8</v>
       </c>
-      <c r="J4" s="32">
+      <c r="J4" s="17">
         <v>5.7200000000000003E-8</v>
       </c>
-      <c r="K4" s="31">
+      <c r="K4" s="16">
         <v>5.7000000000000005E-7</v>
       </c>
       <c r="L4" s="12">
@@ -922,7 +919,7 @@
       <c r="M4" s="14">
         <v>1.312E-5</v>
       </c>
-      <c r="N4" s="19"/>
+      <c r="N4" s="33"/>
     </row>
     <row r="5" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -948,16 +945,16 @@
         <f t="shared" si="0"/>
         <v>1.8974</v>
       </c>
-      <c r="H5" s="33">
+      <c r="H5" s="18">
         <v>1.5299999999999999E-5</v>
       </c>
-      <c r="I5" s="32">
+      <c r="I5" s="17">
         <v>1.85E-7</v>
       </c>
-      <c r="J5" s="32">
+      <c r="J5" s="17">
         <v>1.7700000000000001E-7</v>
       </c>
-      <c r="K5" s="31">
+      <c r="K5" s="16">
         <v>2.7399999999999999E-5</v>
       </c>
       <c r="L5" s="12">
@@ -966,17 +963,17 @@
       <c r="M5" s="14">
         <v>2.4852000000000001E-4</v>
       </c>
-      <c r="N5" s="19"/>
+      <c r="N5" s="33"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>1.7030000000000001</v>
+        <v>2.89</v>
       </c>
       <c r="C6" s="7">
-        <v>2.8919999999999999</v>
+        <v>1.7</v>
       </c>
       <c r="D6" s="7">
         <v>4.9377000000000004</v>
@@ -986,22 +983,22 @@
       </c>
       <c r="F6" s="7">
         <f t="shared" si="1"/>
-        <v>3.2347000000000001</v>
+        <v>2.0477000000000003</v>
       </c>
       <c r="G6" s="8">
         <f t="shared" si="0"/>
-        <v>2.8559999999999999</v>
-      </c>
-      <c r="H6" s="33">
+        <v>1.6639999999999999</v>
+      </c>
+      <c r="H6" s="18">
         <v>7.0999999999999998E-7</v>
       </c>
-      <c r="I6" s="32">
+      <c r="I6" s="17">
         <v>7.1999999999999999E-7</v>
       </c>
-      <c r="J6" s="32">
+      <c r="J6" s="17">
         <v>4.1199999999999998E-7</v>
       </c>
-      <c r="K6" s="31">
+      <c r="K6" s="16">
         <v>5.0399999999999996E-7</v>
       </c>
       <c r="L6" s="12">
@@ -1010,7 +1007,7 @@
       <c r="M6" s="14">
         <v>1.3522999999999999E-4</v>
       </c>
-      <c r="N6" s="20"/>
+      <c r="N6" s="34"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
@@ -1036,16 +1033,16 @@
         <f t="shared" si="0"/>
         <v>0.12490000000000001</v>
       </c>
-      <c r="H7" s="33">
+      <c r="H7" s="18">
         <v>1.1240000000000001E-5</v>
       </c>
-      <c r="I7" s="32">
+      <c r="I7" s="17">
         <v>2.7499999999999999E-6</v>
       </c>
-      <c r="J7" s="32">
+      <c r="J7" s="17">
         <v>2.7999999999999999E-6</v>
       </c>
-      <c r="K7" s="31">
+      <c r="K7" s="16">
         <v>2.9200000000000002E-5</v>
       </c>
       <c r="L7" s="12">
@@ -1054,7 +1051,7 @@
       <c r="M7" s="14">
         <v>1.1299999999999999E-3</v>
       </c>
-      <c r="N7" s="18" t="s">
+      <c r="N7" s="32" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1082,16 +1079,16 @@
         <f t="shared" si="0"/>
         <v>0.29659999999999997</v>
       </c>
-      <c r="H8" s="33">
+      <c r="H8" s="18">
         <v>9.6800000000000005E-6</v>
       </c>
-      <c r="I8" s="32">
+      <c r="I8" s="17">
         <v>7.1999999999999996E-8</v>
       </c>
-      <c r="J8" s="32">
+      <c r="J8" s="17">
         <v>2.0599999999999999E-7</v>
       </c>
-      <c r="K8" s="31">
+      <c r="K8" s="16">
         <v>2.7800000000000001E-5</v>
       </c>
       <c r="L8" s="12">
@@ -1100,7 +1097,7 @@
       <c r="M8" s="14">
         <v>4.9499999999999997E-5</v>
       </c>
-      <c r="N8" s="19"/>
+      <c r="N8" s="33"/>
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
@@ -1126,16 +1123,16 @@
         <f t="shared" si="0"/>
         <v>2.0956000000000001</v>
       </c>
-      <c r="H9" s="33">
+      <c r="H9" s="18">
         <v>2.34E-5</v>
       </c>
-      <c r="I9" s="32">
+      <c r="I9" s="17">
         <v>2.1E-7</v>
       </c>
-      <c r="J9" s="32">
+      <c r="J9" s="17">
         <v>1.8199999999999999E-7</v>
       </c>
-      <c r="K9" s="31">
+      <c r="K9" s="16">
         <v>5.1199999999999998E-5</v>
       </c>
       <c r="L9" s="12">
@@ -1144,17 +1141,17 @@
       <c r="M9" s="14">
         <v>3.7669999999999997E-5</v>
       </c>
-      <c r="N9" s="19"/>
+      <c r="N9" s="33"/>
     </row>
     <row r="10" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="6">
-        <v>1.4490000000000001</v>
+        <v>2.82</v>
       </c>
       <c r="C10" s="7">
-        <v>2.8260000000000001</v>
+        <v>1.44</v>
       </c>
       <c r="D10" s="7">
         <v>4.9409999999999998</v>
@@ -1164,31 +1161,31 @@
       </c>
       <c r="F10" s="7">
         <f t="shared" si="1"/>
-        <v>3.492</v>
+        <v>2.121</v>
       </c>
       <c r="G10" s="8">
         <f t="shared" si="0"/>
-        <v>2.79</v>
-      </c>
-      <c r="H10" s="33">
+        <v>1.4039999999999999</v>
+      </c>
+      <c r="H10" s="18">
         <v>7.5000000000000002E-7</v>
       </c>
-      <c r="I10" s="32">
+      <c r="I10" s="17">
         <v>7.4499999999999996E-7</v>
       </c>
-      <c r="J10" s="32">
+      <c r="J10" s="17">
         <v>4.34E-7</v>
       </c>
-      <c r="K10" s="31">
+      <c r="K10" s="16">
         <v>5.3200000000000005E-7</v>
       </c>
-      <c r="L10" s="34">
+      <c r="L10" s="19">
         <v>2.129E-2</v>
       </c>
-      <c r="M10" s="35">
+      <c r="M10" s="20">
         <v>1.0169E-4</v>
       </c>
-      <c r="N10" s="20"/>
+      <c r="N10" s="34"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -1212,7 +1209,7 @@
       <c r="P12" s="25"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="15" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="10"/>
@@ -1232,7 +1229,7 @@
       <c r="P13" s="28"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C14" s="10"/>
@@ -1244,15 +1241,15 @@
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
-      <c r="M14" s="15" t="s">
+      <c r="M14" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="17"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="31"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="10"/>
@@ -1266,7 +1263,7 @@
       <c r="K15" s="10"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="15" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="10"/>
@@ -1280,7 +1277,7 @@
       <c r="K16" s="10"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C17" s="10"/>
@@ -1294,7 +1291,7 @@
       <c r="K17" s="10"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C18" s="10"/>
@@ -1308,7 +1305,7 @@
       <c r="K18" s="10"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="15" t="s">
         <v>30</v>
       </c>
       <c r="C19" s="10"/>
@@ -1322,7 +1319,7 @@
       <c r="K19" s="10"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C20" s="10"/>

</xml_diff>